<commit_message>
Cleaned the first part of the assignment
</commit_message>
<xml_diff>
--- a/MedicalCentre2.xlsx
+++ b/MedicalCentre2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TD310\OneDrive\Desktop\Everything\Uni Work\GNG5300\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AD9627-A563-4893-BA67-AE8ABE744038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105562AD-F402-4D26-8C92-965B9F35D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="5025" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>PatientId</t>
   </si>
@@ -441,7 +441,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,9 +850,6 @@
       <c r="M9">
         <v>0</v>
       </c>
-      <c r="N9" t="s">
-        <v>29</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Inital draft for part 1
</commit_message>
<xml_diff>
--- a/MedicalCentre2.xlsx
+++ b/MedicalCentre2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TD310\OneDrive\Desktop\Everything\Uni Work\GNG5300\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105562AD-F402-4D26-8C92-965B9F35D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37DA5FC-BD27-4DCE-8627-2832BCD956E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="5025" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4620" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>17</v>
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="s">
         <v>17</v>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" t="s">
         <v>17</v>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completed part A of assignment
</commit_message>
<xml_diff>
--- a/MedicalCentre2.xlsx
+++ b/MedicalCentre2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TD310\OneDrive\Desktop\Everything\Uni Work\GNG5300\Assignments\Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37DA5FC-BD27-4DCE-8627-2832BCD956E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC7F196-7501-4AC0-AF26-97E54A156AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4620" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4770" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>PatientId</t>
   </si>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -651,7 +651,7 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -849,6 +849,50 @@
       </c>
       <c r="M9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>733688164476661</v>
+      </c>
+      <c r="B10">
+        <v>5630279</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>